<commit_message>
Update missing SES values
</commit_message>
<xml_diff>
--- a/badbaby/static/meg_covariates.xlsx
+++ b/badbaby/static/meg_covariates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ss Coding" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3162" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3166" uniqueCount="465">
   <si>
     <t xml:space="preserve">2 months-old</t>
   </si>
@@ -2134,7 +2134,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="V116:V117 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2239,7 +2239,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="V116:V117 B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2460,7 +2460,7 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="V116:V117 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3629,7 +3629,7 @@
     <row r="31" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="35" t="str">
         <f aca="false">" N = "&amp;COUNTA(A2:A30)</f>
-        <v> N = 29</v>
+        <v>N = 29</v>
       </c>
       <c r="B31" s="36" t="str">
         <f aca="false">COUNTIF(B2:B30,"M")&amp;" Males; "&amp;COUNTIF(B2:B30,"F")&amp;" Females"</f>
@@ -4830,7 +4830,7 @@
     <row r="63" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="35" t="str">
         <f aca="false">" N = "&amp;COUNTA(A32:A62)</f>
-        <v> N = 31</v>
+        <v>N = 31</v>
       </c>
       <c r="B63" s="36" t="str">
         <f aca="false">COUNTIF(B32:B62,"M")&amp;" Males; "&amp;COUNTIF(B32:B62,"F")&amp;" Females"</f>
@@ -5661,7 +5661,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
-      <selection pane="bottomRight" activeCell="C85" activeCellId="0" sqref="C85"/>
+      <selection pane="bottomRight" activeCell="C85" activeCellId="1" sqref="V116:V117 C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7977,7 +7977,7 @@
     <row r="54" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="35" t="str">
         <f aca="false">" N = "&amp;COUNTA(A2:A53)</f>
-        <v> N = 52</v>
+        <v>N = 52</v>
       </c>
       <c r="B54" s="37"/>
       <c r="C54" s="37"/>
@@ -8003,23 +8003,23 @@
       </c>
       <c r="I54" s="16" t="str">
         <f aca="false">" N = "&amp;SUM(I2:I53)</f>
-        <v> N = 48</v>
+        <v>N = 48</v>
       </c>
       <c r="J54" s="16" t="str">
         <f aca="false">" N = "&amp;SUM(J2:J53)</f>
-        <v> N = 50</v>
+        <v>N = 50</v>
       </c>
       <c r="K54" s="16" t="str">
         <f aca="false">" N = "&amp;SUM(K2:K53)</f>
-        <v> N = 41</v>
+        <v>N = 41</v>
       </c>
       <c r="L54" s="16" t="str">
         <f aca="false">" N = "&amp;COUNTIF(L2:L53,"3")</f>
-        <v> N = 37</v>
+        <v>N = 37</v>
       </c>
       <c r="M54" s="16" t="str">
         <f aca="false">" N = "&amp;COUNTIF(M2:M53,"TRUE")</f>
-        <v> N = 27</v>
+        <v>N = 27</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9785,7 +9785,7 @@
     <row r="95" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="35" t="str">
         <f aca="false">" N = "&amp;COUNTA(A55:A94)</f>
-        <v> N = 40</v>
+        <v>N = 40</v>
       </c>
       <c r="B95" s="37"/>
       <c r="C95" s="37"/>
@@ -9807,27 +9807,27 @@
       </c>
       <c r="H95" s="16" t="str">
         <f aca="false">" N = "&amp;COUNTIF(H55:H94,"1")</f>
-        <v> N = 33</v>
+        <v>N = 33</v>
       </c>
       <c r="I95" s="16" t="str">
         <f aca="false">" N = "&amp;COUNTIF(I55:I94,"1")</f>
-        <v> N = 40</v>
+        <v>N = 40</v>
       </c>
       <c r="J95" s="16" t="str">
         <f aca="false">" N = "&amp;COUNTIF(J55:J94,"1")</f>
-        <v> N = 38</v>
+        <v>N = 38</v>
       </c>
       <c r="K95" s="16" t="str">
         <f aca="false">" N = "&amp;COUNTIF(K55:K94,"1")</f>
-        <v> N = 33</v>
+        <v>N = 33</v>
       </c>
       <c r="L95" s="16" t="str">
         <f aca="false">" N = "&amp;COUNTIF(L55:L94,"3")</f>
-        <v> N = 32</v>
+        <v>N = 32</v>
       </c>
       <c r="M95" s="16" t="str">
         <f aca="false">" N = "&amp;COUNTIF(M55:M94,"TRUE")</f>
-        <v> N = 26</v>
+        <v>N = 26</v>
       </c>
     </row>
     <row r="65536" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9844,17 +9844,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AH117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J77" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
-      <selection pane="bottomRight" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="V116" activeCellId="0" sqref="V116:V117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9980,7 +9980,7 @@
       <c r="AG1" s="63"/>
       <c r="AH1" s="63"/>
     </row>
-    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="68" t="s">
         <v>59</v>
       </c>
@@ -10069,7 +10069,7 @@
       <c r="AG2" s="70"/>
       <c r="AH2" s="70"/>
     </row>
-    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="68" t="s">
         <v>63</v>
       </c>
@@ -10166,7 +10166,7 @@
       <c r="AG3" s="70"/>
       <c r="AH3" s="70"/>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="68" t="s">
         <v>66</v>
       </c>
@@ -10255,7 +10255,7 @@
       <c r="AG4" s="70"/>
       <c r="AH4" s="70"/>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="68" t="s">
         <v>122</v>
       </c>
@@ -10348,7 +10348,7 @@
       <c r="AG5" s="70"/>
       <c r="AH5" s="70"/>
     </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="68" t="s">
         <v>69</v>
       </c>
@@ -10437,7 +10437,7 @@
       <c r="AG6" s="70"/>
       <c r="AH6" s="70"/>
     </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="68" t="s">
         <v>71</v>
       </c>
@@ -10530,7 +10530,7 @@
       <c r="AG7" s="70"/>
       <c r="AH7" s="70"/>
     </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="68" t="s">
         <v>73</v>
       </c>
@@ -10623,7 +10623,7 @@
       <c r="AG8" s="70"/>
       <c r="AH8" s="70"/>
     </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="68" t="s">
         <v>76</v>
       </c>
@@ -10716,7 +10716,7 @@
       <c r="AG9" s="70"/>
       <c r="AH9" s="70"/>
     </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="68" t="s">
         <v>79</v>
       </c>
@@ -10813,7 +10813,7 @@
       <c r="AG10" s="70"/>
       <c r="AH10" s="70"/>
     </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="68" t="s">
         <v>81</v>
       </c>
@@ -10900,7 +10900,7 @@
       <c r="AG11" s="70"/>
       <c r="AH11" s="70"/>
     </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="68" t="s">
         <v>83</v>
       </c>
@@ -10995,7 +10995,7 @@
       <c r="AG12" s="70"/>
       <c r="AH12" s="70"/>
     </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="68" t="s">
         <v>86</v>
       </c>
@@ -11084,7 +11084,7 @@
       <c r="AG13" s="70"/>
       <c r="AH13" s="70"/>
     </row>
-    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="68" t="s">
         <v>88</v>
       </c>
@@ -11357,7 +11357,7 @@
       <c r="AG16" s="70"/>
       <c r="AH16" s="70"/>
     </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="68" t="s">
         <v>93</v>
       </c>
@@ -11454,7 +11454,7 @@
       <c r="AG17" s="70"/>
       <c r="AH17" s="70"/>
     </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="68" t="s">
         <v>205</v>
       </c>
@@ -11554,7 +11554,7 @@
       <c r="AG18" s="70"/>
       <c r="AH18" s="70"/>
     </row>
-    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="68" t="s">
         <v>95</v>
       </c>
@@ -11831,7 +11831,7 @@
       <c r="AG21" s="70"/>
       <c r="AH21" s="70"/>
     </row>
-    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="68" t="s">
         <v>97</v>
       </c>
@@ -11925,7 +11925,7 @@
       <c r="AG22" s="70"/>
       <c r="AH22" s="70"/>
     </row>
-    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="68" t="s">
         <v>209</v>
       </c>
@@ -12214,7 +12214,7 @@
       <c r="AG25" s="70"/>
       <c r="AH25" s="70"/>
     </row>
-    <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="68" t="s">
         <v>127</v>
       </c>
@@ -12491,7 +12491,7 @@
       <c r="AG28" s="70"/>
       <c r="AH28" s="70"/>
     </row>
-    <row r="29" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="68" t="s">
         <v>104</v>
       </c>
@@ -12584,7 +12584,7 @@
       <c r="AG29" s="70"/>
       <c r="AH29" s="70"/>
     </row>
-    <row r="30" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="68" t="s">
         <v>106</v>
       </c>
@@ -13052,7 +13052,7 @@
       <c r="AG34" s="70"/>
       <c r="AH34" s="70"/>
     </row>
-    <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="68" t="s">
         <v>111</v>
       </c>
@@ -13146,7 +13146,7 @@
       <c r="AG35" s="70"/>
       <c r="AH35" s="70"/>
     </row>
-    <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="68" t="s">
         <v>219</v>
       </c>
@@ -13240,7 +13240,7 @@
       <c r="AG36" s="70"/>
       <c r="AH36" s="70"/>
     </row>
-    <row r="37" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="68" t="s">
         <v>112</v>
       </c>
@@ -13333,7 +13333,7 @@
       <c r="AG37" s="70"/>
       <c r="AH37" s="70"/>
     </row>
-    <row r="38" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="68" t="s">
         <v>220</v>
       </c>
@@ -13617,7 +13617,7 @@
       <c r="AG40" s="70"/>
       <c r="AH40" s="70"/>
     </row>
-    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="68" t="s">
         <v>116</v>
       </c>
@@ -13719,7 +13719,7 @@
       <c r="AG41" s="70"/>
       <c r="AH41" s="70"/>
     </row>
-    <row r="42" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="68" t="s">
         <v>117</v>
       </c>
@@ -13821,7 +13821,7 @@
       <c r="AG42" s="70"/>
       <c r="AH42" s="70"/>
     </row>
-    <row r="43" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="68" t="s">
         <v>224</v>
       </c>
@@ -13923,7 +13923,7 @@
       <c r="AG43" s="70"/>
       <c r="AH43" s="70"/>
     </row>
-    <row r="44" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="68" t="s">
         <v>119</v>
       </c>
@@ -14025,7 +14025,7 @@
       <c r="AG44" s="70"/>
       <c r="AH44" s="70"/>
     </row>
-    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="68" t="s">
         <v>226</v>
       </c>
@@ -14127,7 +14127,7 @@
       <c r="AG45" s="70"/>
       <c r="AH45" s="70"/>
     </row>
-    <row r="46" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="68" t="s">
         <v>128</v>
       </c>
@@ -14223,7 +14223,7 @@
       <c r="AG46" s="70"/>
       <c r="AH46" s="70"/>
     </row>
-    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="68" t="s">
         <v>130</v>
       </c>
@@ -14316,7 +14316,7 @@
       <c r="AG47" s="70"/>
       <c r="AH47" s="70"/>
     </row>
-    <row r="48" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="68" t="s">
         <v>132</v>
       </c>
@@ -14409,7 +14409,7 @@
       <c r="AG48" s="70"/>
       <c r="AH48" s="70"/>
     </row>
-    <row r="49" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="68" t="s">
         <v>133</v>
       </c>
@@ -14500,7 +14500,7 @@
       <c r="AG49" s="70"/>
       <c r="AH49" s="70"/>
     </row>
-    <row r="50" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="68" t="s">
         <v>134</v>
       </c>
@@ -14593,7 +14593,7 @@
       <c r="AG50" s="70"/>
       <c r="AH50" s="70"/>
     </row>
-    <row r="51" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="68" t="s">
         <v>136</v>
       </c>
@@ -14682,7 +14682,7 @@
       <c r="AG51" s="70"/>
       <c r="AH51" s="70"/>
     </row>
-    <row r="52" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="68" t="s">
         <v>228</v>
       </c>
@@ -15148,7 +15148,7 @@
       <c r="AG56" s="70"/>
       <c r="AH56" s="70"/>
     </row>
-    <row r="57" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="68" t="s">
         <v>141</v>
       </c>
@@ -15237,7 +15237,7 @@
       <c r="AG57" s="70"/>
       <c r="AH57" s="70"/>
     </row>
-    <row r="58" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="68" t="s">
         <v>143</v>
       </c>
@@ -15330,7 +15330,7 @@
       <c r="AG58" s="70"/>
       <c r="AH58" s="70"/>
     </row>
-    <row r="59" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="68" t="s">
         <v>145</v>
       </c>
@@ -15599,7 +15599,7 @@
       <c r="AG61" s="70"/>
       <c r="AH61" s="70"/>
     </row>
-    <row r="62" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="68" t="s">
         <v>148</v>
       </c>
@@ -15688,7 +15688,7 @@
       <c r="AG62" s="70"/>
       <c r="AH62" s="70"/>
     </row>
-    <row r="63" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="68" t="s">
         <v>150</v>
       </c>
@@ -15965,7 +15965,7 @@
       <c r="AG65" s="70"/>
       <c r="AH65" s="70"/>
     </row>
-    <row r="66" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="68" t="s">
         <v>153</v>
       </c>
@@ -16599,7 +16599,7 @@
       <c r="AG72" s="70"/>
       <c r="AH72" s="70"/>
     </row>
-    <row r="73" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="68" t="s">
         <v>161</v>
       </c>
@@ -16691,7 +16691,7 @@
       <c r="AG73" s="70"/>
       <c r="AH73" s="70"/>
     </row>
-    <row r="74" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="68" t="s">
         <v>240</v>
       </c>
@@ -16780,7 +16780,7 @@
       <c r="AG74" s="70"/>
       <c r="AH74" s="70"/>
     </row>
-    <row r="75" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="68" t="s">
         <v>162</v>
       </c>
@@ -17049,7 +17049,7 @@
       <c r="AG77" s="70"/>
       <c r="AH77" s="70"/>
     </row>
-    <row r="78" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="68" t="s">
         <v>165</v>
       </c>
@@ -17139,7 +17139,7 @@
       <c r="AG78" s="70"/>
       <c r="AH78" s="70"/>
     </row>
-    <row r="79" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="68" t="s">
         <v>243</v>
       </c>
@@ -17228,7 +17228,7 @@
       <c r="AG79" s="70"/>
       <c r="AH79" s="70"/>
     </row>
-    <row r="80" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="68" t="s">
         <v>166</v>
       </c>
@@ -17318,7 +17318,7 @@
       <c r="AG80" s="70"/>
       <c r="AH80" s="70"/>
     </row>
-    <row r="81" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="68" t="s">
         <v>244</v>
       </c>
@@ -17408,7 +17408,7 @@
       <c r="AG81" s="70"/>
       <c r="AH81" s="70"/>
     </row>
-    <row r="82" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="68" t="s">
         <v>168</v>
       </c>
@@ -17506,7 +17506,7 @@
       <c r="AG82" s="70"/>
       <c r="AH82" s="70"/>
     </row>
-    <row r="83" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="68" t="s">
         <v>246</v>
       </c>
@@ -17606,7 +17606,7 @@
       <c r="AG83" s="70"/>
       <c r="AH83" s="70"/>
     </row>
-    <row r="84" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="68" t="s">
         <v>170</v>
       </c>
@@ -17699,7 +17699,7 @@
       <c r="AG84" s="70"/>
       <c r="AH84" s="70"/>
     </row>
-    <row r="85" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="68" t="s">
         <v>247</v>
       </c>
@@ -17795,7 +17795,7 @@
       <c r="AG85" s="70"/>
       <c r="AH85" s="70"/>
     </row>
-    <row r="86" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="68" t="s">
         <v>187</v>
       </c>
@@ -17892,7 +17892,7 @@
       <c r="AG86" s="70"/>
       <c r="AH86" s="70"/>
     </row>
-    <row r="87" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="68" t="s">
         <v>188</v>
       </c>
@@ -17981,7 +17981,7 @@
       <c r="AG87" s="70"/>
       <c r="AH87" s="70"/>
     </row>
-    <row r="88" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="68" t="s">
         <v>248</v>
       </c>
@@ -18073,7 +18073,7 @@
       <c r="AG88" s="70"/>
       <c r="AH88" s="70"/>
     </row>
-    <row r="89" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="68" t="s">
         <v>171</v>
       </c>
@@ -18167,7 +18167,7 @@
       <c r="AG89" s="70"/>
       <c r="AH89" s="70"/>
     </row>
-    <row r="90" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="68" t="s">
         <v>189</v>
       </c>
@@ -18257,7 +18257,7 @@
       <c r="AG90" s="70"/>
       <c r="AH90" s="70"/>
     </row>
-    <row r="91" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="68" t="s">
         <v>190</v>
       </c>
@@ -18392,7 +18392,7 @@
         <v>1</v>
       </c>
       <c r="M92" s="70" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="N92" s="72" t="n">
         <v>59</v>
@@ -18482,7 +18482,7 @@
         <v>1</v>
       </c>
       <c r="M93" s="70" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="N93" s="72" t="n">
         <v>188</v>
@@ -18572,7 +18572,7 @@
         <v>1</v>
       </c>
       <c r="M94" s="70" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="N94" s="72" t="n">
         <v>64</v>
@@ -18662,7 +18662,7 @@
         <v>1</v>
       </c>
       <c r="M95" s="70" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="N95" s="72" t="n">
         <v>186</v>
@@ -18752,7 +18752,7 @@
         <v>1</v>
       </c>
       <c r="M96" s="70" t="n">
-        <v>0</v>
+        <v>51.5</v>
       </c>
       <c r="N96" s="72" t="n">
         <v>64</v>
@@ -18846,7 +18846,7 @@
         <v>1</v>
       </c>
       <c r="M97" s="70" t="n">
-        <v>0</v>
+        <v>51.5</v>
       </c>
       <c r="N97" s="72" t="n">
         <v>191</v>
@@ -18940,7 +18940,7 @@
         <v>1</v>
       </c>
       <c r="M98" s="70" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="N98" s="72" t="n">
         <v>54</v>
@@ -19034,7 +19034,7 @@
         <v>1</v>
       </c>
       <c r="M99" s="70" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="N99" s="72" t="n">
         <v>188</v>
@@ -19087,7 +19087,7 @@
       <c r="AG99" s="70"/>
       <c r="AH99" s="70"/>
     </row>
-    <row r="100" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="68" t="s">
         <v>173</v>
       </c>
@@ -19176,7 +19176,7 @@
       <c r="AG100" s="70"/>
       <c r="AH100" s="70"/>
     </row>
-    <row r="101" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="68" t="s">
         <v>253</v>
       </c>
@@ -19268,7 +19268,7 @@
       <c r="AG101" s="70"/>
       <c r="AH101" s="70"/>
     </row>
-    <row r="102" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="68" t="s">
         <v>195</v>
       </c>
@@ -19360,7 +19360,7 @@
       <c r="AG102" s="70"/>
       <c r="AH102" s="70"/>
     </row>
-    <row r="103" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="68" t="s">
         <v>255</v>
       </c>
@@ -19449,7 +19449,7 @@
       <c r="AG103" s="70"/>
       <c r="AH103" s="70"/>
     </row>
-    <row r="104" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="68" t="s">
         <v>120</v>
       </c>
@@ -19539,7 +19539,7 @@
       <c r="AG104" s="70"/>
       <c r="AH104" s="70"/>
     </row>
-    <row r="105" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="68" t="s">
         <v>196</v>
       </c>
@@ -19629,7 +19629,7 @@
       <c r="AG105" s="70"/>
       <c r="AH105" s="70"/>
     </row>
-    <row r="106" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="68" t="s">
         <v>256</v>
       </c>
@@ -19719,7 +19719,7 @@
       <c r="AG106" s="70"/>
       <c r="AH106" s="70"/>
     </row>
-    <row r="107" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="68" t="s">
         <v>197</v>
       </c>
@@ -19809,7 +19809,7 @@
       <c r="AG107" s="70"/>
       <c r="AH107" s="70"/>
     </row>
-    <row r="108" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="68" t="s">
         <v>258</v>
       </c>
@@ -19899,7 +19899,7 @@
       <c r="AG108" s="70"/>
       <c r="AH108" s="70"/>
     </row>
-    <row r="109" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="68" t="s">
         <v>198</v>
       </c>
@@ -19989,7 +19989,7 @@
       <c r="AG109" s="70"/>
       <c r="AH109" s="70"/>
     </row>
-    <row r="110" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="68" t="s">
         <v>259</v>
       </c>
@@ -20081,7 +20081,7 @@
       <c r="AG110" s="70"/>
       <c r="AH110" s="70"/>
     </row>
-    <row r="111" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="68" t="s">
         <v>417</v>
       </c>
@@ -20202,7 +20202,7 @@
         <v>1</v>
       </c>
       <c r="M112" s="70" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="N112" s="72" t="n">
         <v>54</v>
@@ -20292,7 +20292,7 @@
         <v>1</v>
       </c>
       <c r="M113" s="70" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="N113" s="72" t="n">
         <v>193</v>
@@ -20341,7 +20341,7 @@
       <c r="AG113" s="70"/>
       <c r="AH113" s="70"/>
     </row>
-    <row r="114" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="68" t="s">
         <v>200</v>
       </c>
@@ -20431,7 +20431,7 @@
       <c r="AG114" s="70"/>
       <c r="AH114" s="70"/>
     </row>
-    <row r="115" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="68" t="s">
         <v>261</v>
       </c>
@@ -20561,7 +20561,7 @@
         <v>1</v>
       </c>
       <c r="M116" s="70" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="N116" s="72" t="n">
         <v>62</v>
@@ -20572,16 +20572,24 @@
       <c r="P116" s="72" t="n">
         <v>40</v>
       </c>
-      <c r="Q116" s="72"/>
+      <c r="Q116" s="72" t="n">
+        <v>16</v>
+      </c>
       <c r="R116" s="72" t="n">
         <v>6</v>
       </c>
-      <c r="S116" s="72"/>
+      <c r="S116" s="72" t="n">
+        <v>18</v>
+      </c>
       <c r="T116" s="72" t="n">
         <v>7</v>
       </c>
-      <c r="U116" s="72"/>
-      <c r="V116" s="72"/>
+      <c r="U116" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="V116" s="72" t="s">
+        <v>362</v>
+      </c>
       <c r="W116" s="72" t="n">
         <v>1</v>
       </c>
@@ -20647,7 +20655,7 @@
         <v>1</v>
       </c>
       <c r="M117" s="70" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="N117" s="72" t="n">
         <v>185</v>
@@ -20658,16 +20666,24 @@
       <c r="P117" s="72" t="n">
         <v>43</v>
       </c>
-      <c r="Q117" s="72"/>
+      <c r="Q117" s="72" t="n">
+        <v>16</v>
+      </c>
       <c r="R117" s="72" t="n">
         <v>6</v>
       </c>
-      <c r="S117" s="72"/>
+      <c r="S117" s="72" t="n">
+        <v>18</v>
+      </c>
       <c r="T117" s="72" t="n">
         <v>7</v>
       </c>
-      <c r="U117" s="72"/>
-      <c r="V117" s="72"/>
+      <c r="U117" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="V117" s="72" t="s">
+        <v>362</v>
+      </c>
       <c r="W117" s="72" t="n">
         <v>1</v>
       </c>
@@ -20693,7 +20709,13 @@
       <c r="AH117" s="70"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AF117"/>
+  <autoFilter ref="A1:AF117">
+    <filterColumn colId="11">
+      <customFilters and="true">
+        <customFilter operator="equal" val="1"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -20713,18 +20735,18 @@
   <dimension ref="A1:AMJ117"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="V116:V117 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="80" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="80" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="80" width="13.37"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="6" style="80" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="80" width="15.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="13" style="80" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="81" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="81" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="81" width="17.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="23" style="80" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="62" width="11.52"/>
   </cols>
@@ -29319,8 +29341,8 @@
   </sheetPr>
   <dimension ref="A1:AA117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A68" activeCellId="1" sqref="V116:V117 A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34713,8 +34735,8 @@
   </sheetPr>
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F94" activeCellId="0" sqref="F94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F94" activeCellId="1" sqref="V116:V117 F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36613,7 +36635,7 @@
   <dimension ref="A1:Y117"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
+      <selection pane="topLeft" activeCell="A87" activeCellId="1" sqref="V116:V117 A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>